<commit_message>
github spinnt, ich hab nur bei mir was geändert
</commit_message>
<xml_diff>
--- a/German_Tales/Data/org/Firmenich_Inhalt_Bd4.xlsx
+++ b/German_Tales/Data/org/Firmenich_Inhalt_Bd4.xlsx
@@ -1,21 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/81aa60b0b6324d95/Dokumente/GitHub/DWA/German_Tales/Data/org/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_E3FCB1C26D9788B9817A6E9C558403E634C5C93A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E044264D-CB6B-4CA2-955B-7886742E1C56}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Tabelle2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Tabelle3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
+    <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="137">
   <si>
     <t>Bd.</t>
   </si>
@@ -35,7 +42,7 @@
     <t>Titel</t>
   </si>
   <si>
-    <t xml:space="preserve">ggf. Titel</t>
+    <t>ggf. Titel</t>
   </si>
   <si>
     <t>Reim</t>
@@ -53,10 +60,10 @@
     <t>y</t>
   </si>
   <si>
-    <t xml:space="preserve">Bemerkung Erfassung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mundart in Halland. Mundart in den Södra-Fjäre= und Biske-Bezirken.</t>
+    <t>Bemerkung Erfassung</t>
+  </si>
+  <si>
+    <t>Mundart in Halland. Mundart in den Södra-Fjäre= und Biske-Bezirken.</t>
   </si>
   <si>
     <t>Halland</t>
@@ -71,7 +78,7 @@
     <t>11.9840433</t>
   </si>
   <si>
-    <t xml:space="preserve">Mundart in dem Himle-Bezirk.</t>
+    <t>Mundart in dem Himle-Bezirk.</t>
   </si>
   <si>
     <t>Himle</t>
@@ -83,7 +90,7 @@
     <t>12.3438859</t>
   </si>
   <si>
-    <t xml:space="preserve">Mundart in dem Faurås-Bezirk.</t>
+    <t>Mundart in dem Faurås-Bezirk.</t>
   </si>
   <si>
     <t>Faurås</t>
@@ -95,22 +102,22 @@
     <t>12.5463262</t>
   </si>
   <si>
-    <t xml:space="preserve">Mundart in den Tönnersjö= und Höks=Bezirken.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tönnersjö, Höks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">56.6421671, 56.6628238</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13.0491471, 12.9066077</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mundart in Westgothland.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Västra Götalands län</t>
+    <t>Mundart in den Tönnersjö= und Höks=Bezirken.</t>
+  </si>
+  <si>
+    <t>Tönnersjö, Höks</t>
+  </si>
+  <si>
+    <t>56.6421671, 56.6628238</t>
+  </si>
+  <si>
+    <t>13.0491471, 12.9066077</t>
+  </si>
+  <si>
+    <t>Mundart in Westgothland.</t>
+  </si>
+  <si>
+    <t>Västra Götalands län</t>
   </si>
   <si>
     <t>j</t>
@@ -122,10 +129,10 @@
     <t>10.0504282</t>
   </si>
   <si>
-    <t xml:space="preserve">Mundart in dem Kirchspiel Stora Mellösa in der Provinz Nerike in Schweden.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stora Mellösa</t>
+    <t>Mundart in dem Kirchspiel Stora Mellösa in der Provinz Nerike in Schweden.</t>
+  </si>
+  <si>
+    <t>Stora Mellösa</t>
   </si>
   <si>
     <t>59.2119546</t>
@@ -134,7 +141,7 @@
     <t>15.4781718</t>
   </si>
   <si>
-    <t xml:space="preserve">Mundart in dem Kirchspiel Delsbo im nördlichen Helsingland.</t>
+    <t>Mundart in dem Kirchspiel Delsbo im nördlichen Helsingland.</t>
   </si>
   <si>
     <t>Delsbo</t>
@@ -149,10 +156,10 @@
     <t>16.4795635</t>
   </si>
   <si>
-    <t xml:space="preserve">Text beginnt in Prosa-Form, später sind Reime vorhanden.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Skellefte- und Norsjö-Mundart im Vesterbotten (Westboden) im nördlichsten Theile Schwedens.</t>
+    <t>Text beginnt in Prosa-Form, später sind Reime vorhanden.</t>
+  </si>
+  <si>
+    <t>Skellefte- und Norsjö-Mundart im Vesterbotten (Westboden) im nördlichsten Theile Schwedens.</t>
   </si>
   <si>
     <t>Västerbotten</t>
@@ -164,7 +171,7 @@
     <t>12.8363292</t>
   </si>
   <si>
-    <t xml:space="preserve">Mundart in dem Kirchspiel Nerpes im Oesterbotten (Ostboden) im Nyland des Großfürstenthums Finnland.</t>
+    <t>Mundart in dem Kirchspiel Nerpes im Oesterbotten (Ostboden) im Nyland des Großfürstenthums Finnland.</t>
   </si>
   <si>
     <t>Närpes</t>
@@ -176,7 +183,7 @@
     <t>21.316553</t>
   </si>
   <si>
-    <t xml:space="preserve">Mundart in dem Kirchspiel Kronoby im Oesterbotten (Ostboden) im Nyland des Großfürstenthums Finnland.</t>
+    <t>Mundart in dem Kirchspiel Kronoby im Oesterbotten (Ostboden) im Nyland des Großfürstenthums Finnland.</t>
   </si>
   <si>
     <t>Kronoby</t>
@@ -188,7 +195,7 @@
     <t>23.0131466</t>
   </si>
   <si>
-    <t xml:space="preserve">Mundart in Gamla Karleby im Oesterbotten (Ostboden) im Nyland des Großfürstenthums Finnland.</t>
+    <t>Mundart in Gamla Karleby im Oesterbotten (Ostboden) im Nyland des Großfürstenthums Finnland.</t>
   </si>
   <si>
     <t>Kokkola</t>
@@ -203,7 +210,7 @@
     <t xml:space="preserve">Anmerkung zum Ort: Gamlakarleby wurde 1976 in 'Kokkola' umbenannt. </t>
   </si>
   <si>
-    <t xml:space="preserve">Mundart in dem Kirchspiel Ny-Karleby im Oesterbotten (Ostboden) in Nyland des Großfürstenthums Finnland.</t>
+    <t>Mundart in dem Kirchspiel Ny-Karleby im Oesterbotten (Ostboden) in Nyland des Großfürstenthums Finnland.</t>
   </si>
   <si>
     <t>Nykarleby</t>
@@ -215,7 +222,7 @@
     <t>22.5128463</t>
   </si>
   <si>
-    <t xml:space="preserve">Mundart in dem Kirchspiel Pedersöre im Oesterbotten (Ostboden) im Nyland des Großfürstenthums Finnland.</t>
+    <t>Mundart in dem Kirchspiel Pedersöre im Oesterbotten (Ostboden) im Nyland des Großfürstenthums Finnland.</t>
   </si>
   <si>
     <t>Pedersöre</t>
@@ -227,7 +234,7 @@
     <t>22.7230908</t>
   </si>
   <si>
-    <t xml:space="preserve">Mundart im mittelsten Theile des Kirchspiels Ingå im Nyland des Großfürstenthums Finnland.</t>
+    <t>Mundart im mittelsten Theile des Kirchspiels Ingå im Nyland des Großfürstenthums Finnland.</t>
   </si>
   <si>
     <t>Ingå</t>
@@ -239,13 +246,13 @@
     <t>23.9666971</t>
   </si>
   <si>
-    <t xml:space="preserve">Altschwedische Sprache im vierzehnten Jahrhundert.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[kein Ort angegeben]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Schwedische Schriftsprache.</t>
+    <t>Altschwedische Sprache im vierzehnten Jahrhundert.</t>
+  </si>
+  <si>
+    <t>[kein Ort angegeben]</t>
+  </si>
+  <si>
+    <t>Schwedische Schriftsprache.</t>
   </si>
   <si>
     <t>Schweden</t>
@@ -257,13 +264,13 @@
     <t>-3.3114366</t>
   </si>
   <si>
-    <t xml:space="preserve">Frage: Koordinaten von 'Schweden' angeben?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nachträge zu den dänischen Mundarten. Mundart der Gegend westlich von Holbäk auf Seeland.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Svinninge (westlich von Holbæk)</t>
+    <t>Frage: Koordinaten von 'Schweden' angeben?</t>
+  </si>
+  <si>
+    <t>Nachträge zu den dänischen Mundarten. Mundart der Gegend westlich von Holbäk auf Seeland.</t>
+  </si>
+  <si>
+    <t>Svinninge (westlich von Holbæk)</t>
   </si>
   <si>
     <t>55.7314396</t>
@@ -272,10 +279,10 @@
     <t>11.4017269</t>
   </si>
   <si>
-    <t xml:space="preserve">Das eigentliche Kapitel beginnt auf S. 24 mit Vorbemerkungen zur Aussprache./ + Svinninge als Ort gewählt. Svinninge ist der nächstgelegene Ort westlich von Holbæk auf Seeland.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mundart auf Seeland.</t>
+    <t>Das eigentliche Kapitel beginnt auf S. 24 mit Vorbemerkungen zur Aussprache./ + Svinninge als Ort gewählt. Svinninge ist der nächstgelegene Ort westlich von Holbæk auf Seeland.</t>
+  </si>
+  <si>
+    <t>Mundart auf Seeland.</t>
   </si>
   <si>
     <t>Seeland</t>
@@ -287,7 +294,7 @@
     <t>10.4306388</t>
   </si>
   <si>
-    <t xml:space="preserve">Mundart des Fischerdorfes Hesnäs auf Falster.</t>
+    <t>Mundart des Fischerdorfes Hesnäs auf Falster.</t>
   </si>
   <si>
     <t>Hesnæs</t>
@@ -299,10 +306,10 @@
     <t>12.1157744</t>
   </si>
   <si>
-    <t xml:space="preserve">Das eigentliche Kapitel beginnt auf S. 26 mit Vorbemerkungen über die Aussprache.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Altdänische Sprache im vierzehnten Jahrhundert.</t>
+    <t>Das eigentliche Kapitel beginnt auf S. 26 mit Vorbemerkungen über die Aussprache.</t>
+  </si>
+  <si>
+    <t>Altdänische Sprache im vierzehnten Jahrhundert.</t>
   </si>
   <si>
     <t>Kalmar</t>
@@ -314,7 +321,7 @@
     <t>16.2453884</t>
   </si>
   <si>
-    <t xml:space="preserve">Alte isländische Lieder.</t>
+    <t>Alte isländische Lieder.</t>
   </si>
   <si>
     <t>Island</t>
@@ -329,10 +336,10 @@
     <t xml:space="preserve">Frage: Koordinaten von 'Island' angeben? + Quellenangabe und Erläuterungstext in der Kapitelüberschrift, gilt also für alle Texte. </t>
   </si>
   <si>
-    <t xml:space="preserve">Alte isländische Sprache oder Sprache der Edda.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Altnordische Sprache im zehnten Jahrhundert.</t>
+    <t>Alte isländische Sprache oder Sprache der Edda.</t>
+  </si>
+  <si>
+    <t>Altnordische Sprache im zehnten Jahrhundert.</t>
   </si>
   <si>
     <t>Dänemark</t>
@@ -344,10 +351,10 @@
     <t>6.2617775</t>
   </si>
   <si>
-    <t xml:space="preserve">Dänemark als Ort in der Fußnote angegeben.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mundart der Bewohner der Färöer.</t>
+    <t>Dänemark als Ort in der Fußnote angegeben.</t>
+  </si>
+  <si>
+    <t>Mundart der Bewohner der Färöer.</t>
   </si>
   <si>
     <t>Färöer</t>
@@ -359,10 +366,10 @@
     <t>-9.3200063</t>
   </si>
   <si>
-    <t xml:space="preserve">Vorbemerkungen zum Text vorhanden.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nachträge zu den Norwegischen Mundarten. Mundart in Stjördalen im Stifte Trondhjem.</t>
+    <t>Vorbemerkungen zum Text vorhanden.</t>
+  </si>
+  <si>
+    <t>Nachträge zu den Norwegischen Mundarten. Mundart in Stjördalen im Stifte Trondhjem.</t>
   </si>
   <si>
     <t>Trondheim</t>
@@ -374,10 +381,10 @@
     <t>10.257752</t>
   </si>
   <si>
-    <t xml:space="preserve">Mundart in Örkedalen im Stifte Trondhjem.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mundart auf Nordmör im Stifte Trondhjem</t>
+    <t>Mundart in Örkedalen im Stifte Trondhjem.</t>
+  </si>
+  <si>
+    <t>Mundart auf Nordmör im Stifte Trondhjem</t>
   </si>
   <si>
     <t>Nordmøre</t>
@@ -389,7 +396,7 @@
     <t>5.552531</t>
   </si>
   <si>
-    <t xml:space="preserve">Mundart an dem Trondhjemsfjord.</t>
+    <t>Mundart an dem Trondhjemsfjord.</t>
   </si>
   <si>
     <t>Trondheimsfjorden</t>
@@ -401,13 +408,13 @@
     <t>5.6028944</t>
   </si>
   <si>
-    <t xml:space="preserve">Altnorwegische Sprache</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Das eigentliche Kapitel beginnt auf S. 80 mit Vorbemerkungen.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allgemeine norwegische Sprache.</t>
+    <t>Altnorwegische Sprache</t>
+  </si>
+  <si>
+    <t>Das eigentliche Kapitel beginnt auf S. 80 mit Vorbemerkungen.</t>
+  </si>
+  <si>
+    <t>Allgemeine norwegische Sprache.</t>
   </si>
   <si>
     <t>Norwegen</t>
@@ -419,10 +426,10 @@
     <t>-2.9171951</t>
   </si>
   <si>
-    <t xml:space="preserve">Frage: Norwegen als Ort angeben?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alte angelsächsische Sprache.</t>
+    <t>Frage: Norwegen als Ort angeben?</t>
+  </si>
+  <si>
+    <t>Alte angelsächsische Sprache.</t>
   </si>
   <si>
     <t>ENDE</t>
@@ -431,17 +438,17 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11.000000"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11.000000"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
@@ -465,18 +472,13 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="3" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -487,295 +489,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="1F497D"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="EEECE1"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4F81BD"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="C0504D"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="9BBB59"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8064A2"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4BACC6"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="F79646"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000FF"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="800080"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Angsana New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Cordia New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-</a:theme>
-</file>
-
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -980,30 +702,32 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M124"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" zoomScale="100" workbookViewId="0">
-      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="36.57421875"/>
-    <col customWidth="1" min="3" max="3" width="18.140625"/>
-    <col customWidth="1" min="6" max="6" width="78.140625"/>
-    <col customWidth="1" min="7" max="7" width="58.421875"/>
-    <col customWidth="1" min="9" max="9" width="18.28125"/>
-    <col customWidth="1" min="10" max="10" width="18.140625"/>
-    <col customWidth="1" min="11" max="11" width="24.8515625"/>
-    <col customWidth="1" min="12" max="12" width="27.57421875"/>
-    <col customWidth="1" min="13" max="13" width="27.140625"/>
+    <col min="2" max="2" width="52.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="6" max="6" width="78.140625" customWidth="1"/>
+    <col min="7" max="7" width="58.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" customWidth="1"/>
+    <col min="11" max="11" width="24.85546875" customWidth="1"/>
+    <col min="12" max="12" width="27.5703125" customWidth="1"/>
+    <col min="13" max="13" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1044,7 +768,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" ht="14.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>4</v>
       </c>
@@ -1076,7 +800,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" ht="14.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>4</v>
       </c>
@@ -1108,14 +832,14 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" ht="14.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s">
         <v>23</v>
       </c>
       <c r="D4">
@@ -1133,14 +857,14 @@
       <c r="J4" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="L4" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" ht="14.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1172,7 +896,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" ht="14.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1200,11 +924,11 @@
       <c r="K6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L6" s="4" t="s">
+      <c r="L6" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7" ht="14.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -1229,14 +953,14 @@
       <c r="J7" t="s">
         <v>32</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="K7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="L7" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="8" ht="14.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -1261,17 +985,17 @@
       <c r="J8" t="s">
         <v>32</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="K8" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="L8" s="4" t="s">
+      <c r="L8" s="2" t="s">
         <v>43</v>
       </c>
       <c r="M8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="9" ht="14.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
@@ -1296,14 +1020,14 @@
       <c r="J9" t="s">
         <v>32</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="K9" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="L9" s="4" t="s">
+      <c r="L9" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="10" ht="14.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4</v>
       </c>
@@ -1328,14 +1052,14 @@
       <c r="J10" t="s">
         <v>32</v>
       </c>
-      <c r="K10" s="4" t="s">
+      <c r="K10" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="L10" s="4" t="s">
+      <c r="L10" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" ht="14.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4</v>
       </c>
@@ -1360,14 +1084,14 @@
       <c r="J11" t="s">
         <v>32</v>
       </c>
-      <c r="K11" s="4" t="s">
+      <c r="K11" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="L11" s="4" t="s">
+      <c r="L11" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="12" ht="14.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>4</v>
       </c>
@@ -1392,17 +1116,17 @@
       <c r="J12" t="s">
         <v>32</v>
       </c>
-      <c r="K12" s="4" t="s">
+      <c r="K12" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="L12" s="4" t="s">
+      <c r="L12" s="2" t="s">
         <v>60</v>
       </c>
       <c r="M12" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="13" ht="14.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4</v>
       </c>
@@ -1412,14 +1136,12 @@
       <c r="C13" t="s">
         <v>58</v>
       </c>
-      <c r="D13" s="5">
-        <v>15</v>
-      </c>
-      <c r="E13" s="5">
+      <c r="D13">
+        <v>15</v>
+      </c>
+      <c r="E13">
         <v>18</v>
       </c>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
       <c r="H13" t="s">
         <v>15</v>
       </c>
@@ -1429,14 +1151,14 @@
       <c r="J13" t="s">
         <v>32</v>
       </c>
-      <c r="K13" s="4" t="s">
+      <c r="K13" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="L13" s="4" t="s">
+      <c r="L13" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="14" ht="14.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>4</v>
       </c>
@@ -1461,14 +1183,14 @@
       <c r="J14" t="s">
         <v>32</v>
       </c>
-      <c r="K14" s="4" t="s">
+      <c r="K14" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="L14" s="4" t="s">
+      <c r="L14" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="15" ht="14.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>4</v>
       </c>
@@ -1493,14 +1215,14 @@
       <c r="J15" t="s">
         <v>32</v>
       </c>
-      <c r="K15" s="4" t="s">
+      <c r="K15" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="L15" s="4" t="s">
+      <c r="L15" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="16" ht="14.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>4</v>
       </c>
@@ -1525,14 +1247,14 @@
       <c r="J16" t="s">
         <v>15</v>
       </c>
-      <c r="K16" s="4" t="s">
+      <c r="K16" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="L16" s="4" t="s">
+      <c r="L16" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="17" ht="14.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>4</v>
       </c>
@@ -1564,7 +1286,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="18" ht="14.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>4</v>
       </c>
@@ -1589,34 +1311,32 @@
       <c r="J18" t="s">
         <v>32</v>
       </c>
-      <c r="K18" s="4" t="s">
+      <c r="K18" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="L18" s="4" t="s">
+      <c r="L18" s="2" t="s">
         <v>79</v>
       </c>
       <c r="M18" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="19" ht="14.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>4</v>
       </c>
       <c r="B19" t="s">
         <v>76</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" t="s">
         <v>77</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19">
         <v>22</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19">
         <v>22</v>
       </c>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
       <c r="H19" t="s">
         <v>32</v>
       </c>
@@ -1626,34 +1346,29 @@
       <c r="J19" t="s">
         <v>32</v>
       </c>
-      <c r="K19" s="4" t="s">
+      <c r="K19" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="L19" s="4" t="s">
+      <c r="L19" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="M19"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="5"/>
-    </row>
-    <row r="20" ht="14.25">
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>4</v>
       </c>
       <c r="B20" t="s">
         <v>76</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" t="s">
         <v>77</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20">
         <v>23</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20">
         <v>23</v>
       </c>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
       <c r="H20" t="s">
         <v>32</v>
       </c>
@@ -1663,17 +1378,14 @@
       <c r="J20" t="s">
         <v>32</v>
       </c>
-      <c r="K20" s="4" t="s">
+      <c r="K20" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="L20" s="4" t="s">
+      <c r="L20" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="M20"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="5"/>
-    </row>
-    <row r="21" ht="14.25">
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>4</v>
       </c>
@@ -1698,17 +1410,17 @@
       <c r="J21" t="s">
         <v>32</v>
       </c>
-      <c r="K21" s="4" t="s">
+      <c r="K21" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="L21" s="4" t="s">
+      <c r="L21" s="2" t="s">
         <v>84</v>
       </c>
       <c r="M21" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="22" ht="14.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>4</v>
       </c>
@@ -1733,14 +1445,14 @@
       <c r="J22" t="s">
         <v>15</v>
       </c>
-      <c r="K22" s="4" t="s">
+      <c r="K22" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="L22" s="4" t="s">
+      <c r="L22" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="23" ht="14.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>4</v>
       </c>
@@ -1765,17 +1477,17 @@
       <c r="J23" t="s">
         <v>32</v>
       </c>
-      <c r="K23" s="4" t="s">
+      <c r="K23" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="L23" s="4" t="s">
+      <c r="L23" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="M23" s="3" t="s">
+      <c r="M23" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="24" ht="14.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>4</v>
       </c>
@@ -1800,14 +1512,14 @@
       <c r="J24" t="s">
         <v>32</v>
       </c>
-      <c r="K24" s="4" t="s">
+      <c r="K24" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="L24" s="4" t="s">
+      <c r="L24" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="25" ht="14.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>4</v>
       </c>
@@ -1832,17 +1544,17 @@
       <c r="J25" t="s">
         <v>32</v>
       </c>
-      <c r="K25" s="4" t="s">
+      <c r="K25" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="L25" s="4" t="s">
+      <c r="L25" s="2" t="s">
         <v>102</v>
       </c>
       <c r="M25" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="26" ht="14.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>4</v>
       </c>
@@ -1867,14 +1579,14 @@
       <c r="J26" t="s">
         <v>32</v>
       </c>
-      <c r="K26" s="4" t="s">
+      <c r="K26" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="L26" s="4" t="s">
+      <c r="L26" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="27" ht="14.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>4</v>
       </c>
@@ -1899,14 +1611,14 @@
       <c r="J27" t="s">
         <v>32</v>
       </c>
-      <c r="K27" s="4" t="s">
+      <c r="K27" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="L27" s="4" t="s">
+      <c r="L27" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="28" ht="14.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>4</v>
       </c>
@@ -1931,14 +1643,14 @@
       <c r="J28" t="s">
         <v>32</v>
       </c>
-      <c r="K28" s="4" t="s">
+      <c r="K28" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="L28" s="4" t="s">
+      <c r="L28" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="29" ht="14.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>4</v>
       </c>
@@ -1963,14 +1675,14 @@
       <c r="J29" t="s">
         <v>32</v>
       </c>
-      <c r="K29" s="4" t="s">
+      <c r="K29" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="L29" s="4" t="s">
+      <c r="L29" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="30" ht="14.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>4</v>
       </c>
@@ -1995,14 +1707,14 @@
       <c r="J30" t="s">
         <v>32</v>
       </c>
-      <c r="K30" s="4" t="s">
+      <c r="K30" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="L30" s="4" t="s">
+      <c r="L30" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="31" ht="14.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>4</v>
       </c>
@@ -2027,14 +1739,14 @@
       <c r="J31" t="s">
         <v>32</v>
       </c>
-      <c r="K31" s="4" t="s">
+      <c r="K31" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="L31" s="4" t="s">
+      <c r="L31" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="32" ht="14.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>4</v>
       </c>
@@ -2059,14 +1771,14 @@
       <c r="J32" t="s">
         <v>32</v>
       </c>
-      <c r="K32" s="4" t="s">
+      <c r="K32" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="L32" s="4" t="s">
+      <c r="L32" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="33" ht="14.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>4</v>
       </c>
@@ -2091,14 +1803,14 @@
       <c r="J33" t="s">
         <v>32</v>
       </c>
-      <c r="K33" s="4" t="s">
+      <c r="K33" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="L33" s="4" t="s">
+      <c r="L33" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="34" ht="14.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>4</v>
       </c>
@@ -2123,21 +1835,21 @@
       <c r="J34" t="s">
         <v>32</v>
       </c>
-      <c r="K34" s="4" t="s">
+      <c r="K34" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="L34" s="4" t="s">
+      <c r="L34" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="35" ht="14.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>4</v>
       </c>
       <c r="B35" t="s">
         <v>104</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="2" t="s">
         <v>75</v>
       </c>
       <c r="D35">
@@ -2158,11 +1870,11 @@
       <c r="K35" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="L35" s="4" t="s">
+      <c r="L35" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="36" ht="14.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>4</v>
       </c>
@@ -2187,17 +1899,17 @@
       <c r="J36" t="s">
         <v>15</v>
       </c>
-      <c r="K36" s="4" t="s">
+      <c r="K36" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="L36" s="4" t="s">
+      <c r="L36" s="2" t="s">
         <v>108</v>
       </c>
       <c r="M36" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="37" ht="14.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>4</v>
       </c>
@@ -2222,14 +1934,14 @@
       <c r="J37" t="s">
         <v>32</v>
       </c>
-      <c r="K37" s="4" t="s">
+      <c r="K37" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="L37" s="4" t="s">
+      <c r="L37" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="38" ht="14.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>4</v>
       </c>
@@ -2254,14 +1966,14 @@
       <c r="J38" t="s">
         <v>32</v>
       </c>
-      <c r="K38" s="4" t="s">
+      <c r="K38" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="L38" s="4" t="s">
+      <c r="L38" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="39" ht="14.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>4</v>
       </c>
@@ -2286,14 +1998,14 @@
       <c r="J39" t="s">
         <v>32</v>
       </c>
-      <c r="K39" s="4" t="s">
+      <c r="K39" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="L39" s="4" t="s">
+      <c r="L39" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="40" ht="14.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>4</v>
       </c>
@@ -2318,14 +2030,14 @@
       <c r="J40" t="s">
         <v>32</v>
       </c>
-      <c r="K40" s="4" t="s">
+      <c r="K40" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="L40" s="4" t="s">
+      <c r="L40" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="41" ht="14.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>4</v>
       </c>
@@ -2350,14 +2062,14 @@
       <c r="J41" t="s">
         <v>32</v>
       </c>
-      <c r="K41" s="4" t="s">
+      <c r="K41" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="L41" s="4" t="s">
+      <c r="L41" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="42" ht="14.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>4</v>
       </c>
@@ -2382,14 +2094,14 @@
       <c r="J42" t="s">
         <v>32</v>
       </c>
-      <c r="K42" s="4" t="s">
+      <c r="K42" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="L42" s="4" t="s">
+      <c r="L42" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="43" ht="14.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>4</v>
       </c>
@@ -2414,17 +2126,17 @@
       <c r="J43" t="s">
         <v>32</v>
       </c>
-      <c r="K43" s="4" t="s">
+      <c r="K43" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="L43" s="4" t="s">
+      <c r="L43" s="2" t="s">
         <v>113</v>
       </c>
       <c r="M43" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="44" ht="14.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>4</v>
       </c>
@@ -2449,14 +2161,14 @@
       <c r="J44" t="s">
         <v>32</v>
       </c>
-      <c r="K44" s="4" t="s">
+      <c r="K44" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="L44" s="4" t="s">
+      <c r="L44" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="45" ht="14.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>4</v>
       </c>
@@ -2481,14 +2193,14 @@
       <c r="J45" t="s">
         <v>15</v>
       </c>
-      <c r="K45" s="4" t="s">
+      <c r="K45" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="L45" s="4" t="s">
+      <c r="L45" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="46" ht="14.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>4</v>
       </c>
@@ -2513,14 +2225,14 @@
       <c r="J46" t="s">
         <v>15</v>
       </c>
-      <c r="K46" s="4" t="s">
+      <c r="K46" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="L46" s="4" t="s">
+      <c r="L46" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="47" ht="14.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>4</v>
       </c>
@@ -2545,14 +2257,14 @@
       <c r="J47" t="s">
         <v>15</v>
       </c>
-      <c r="K47" s="4" t="s">
+      <c r="K47" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="L47" s="4" t="s">
+      <c r="L47" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="48" ht="14.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>4</v>
       </c>
@@ -2577,14 +2289,14 @@
       <c r="J48" t="s">
         <v>32</v>
       </c>
-      <c r="K48" s="4" t="s">
+      <c r="K48" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="L48" s="4" t="s">
+      <c r="L48" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="49" ht="14.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>4</v>
       </c>
@@ -2609,17 +2321,17 @@
       <c r="J49" t="s">
         <v>32</v>
       </c>
-      <c r="K49" s="4" t="s">
+      <c r="K49" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="L49" s="4" t="s">
+      <c r="L49" s="2" t="s">
         <v>75</v>
       </c>
       <c r="M49" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="50" ht="14.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>4</v>
       </c>
@@ -2644,17 +2356,17 @@
       <c r="J50" t="s">
         <v>32</v>
       </c>
-      <c r="K50" s="4" t="s">
+      <c r="K50" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="L50" s="4" t="s">
+      <c r="L50" s="2" t="s">
         <v>133</v>
       </c>
       <c r="M50" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="51" ht="14.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>4</v>
       </c>
@@ -2686,336 +2398,328 @@
         <v>75</v>
       </c>
     </row>
-    <row r="52" ht="14.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>136</v>
       </c>
-      <c r="K52" s="4"/>
-      <c r="L52" s="4"/>
-    </row>
-    <row r="53" ht="14.25">
-      <c r="K53" s="4"/>
-      <c r="L53" s="4"/>
-    </row>
-    <row r="54" ht="14.25">
-      <c r="K54" s="4"/>
-      <c r="L54" s="4"/>
-    </row>
-    <row r="55" ht="14.25">
-      <c r="K55" s="4"/>
-      <c r="L55" s="4"/>
-    </row>
-    <row r="56" ht="14.25">
-      <c r="K56" s="4"/>
-      <c r="L56" s="4"/>
-    </row>
-    <row r="57" ht="14.25">
-      <c r="K57" s="4"/>
-      <c r="L57" s="4"/>
-    </row>
-    <row r="58" ht="14.25">
-      <c r="K58" s="4"/>
-      <c r="L58" s="4"/>
-    </row>
-    <row r="59" ht="14.25">
-      <c r="K59" s="4"/>
-      <c r="L59" s="4"/>
-    </row>
-    <row r="60" ht="14.25">
-      <c r="K60" s="4"/>
-      <c r="L60" s="4"/>
-    </row>
-    <row r="61" ht="14.25">
-      <c r="K61" s="4"/>
-      <c r="L61" s="4"/>
-    </row>
-    <row r="62" ht="14.25">
-      <c r="K62" s="4"/>
-      <c r="L62" s="4"/>
-    </row>
-    <row r="63" ht="14.25">
-      <c r="K63" s="4"/>
-      <c r="L63" s="4"/>
-    </row>
-    <row r="64" ht="14.25">
-      <c r="K64" s="4"/>
-      <c r="L64" s="4"/>
-    </row>
-    <row r="65" ht="14.25">
-      <c r="K65" s="4"/>
-      <c r="L65" s="4"/>
-    </row>
-    <row r="66" ht="14.25">
-      <c r="K66" s="4"/>
-      <c r="L66" s="4"/>
-    </row>
-    <row r="67" ht="14.25">
-      <c r="K67" s="4"/>
-      <c r="L67" s="4"/>
-    </row>
-    <row r="68" ht="14.25">
-      <c r="K68" s="4"/>
-      <c r="L68" s="4"/>
-    </row>
-    <row r="69" ht="14.25">
-      <c r="K69" s="4"/>
-      <c r="L69" s="4"/>
-    </row>
-    <row r="70" ht="14.25">
-      <c r="K70" s="4"/>
-      <c r="L70" s="4"/>
-    </row>
-    <row r="71" ht="14.25">
-      <c r="K71" s="4"/>
-      <c r="L71" s="4"/>
-    </row>
-    <row r="72" ht="14.25">
-      <c r="K72" s="4"/>
-      <c r="L72" s="4"/>
-    </row>
-    <row r="73" ht="14.25">
-      <c r="K73" s="4"/>
-      <c r="L73" s="4"/>
-    </row>
-    <row r="74" ht="14.25">
-      <c r="K74" s="4"/>
-      <c r="L74" s="4"/>
-    </row>
-    <row r="75" ht="14.25">
-      <c r="K75" s="4"/>
-      <c r="L75" s="4"/>
-    </row>
-    <row r="76" ht="14.25">
-      <c r="K76" s="4"/>
-      <c r="L76" s="4"/>
-    </row>
-    <row r="77" ht="14.25">
-      <c r="K77" s="4"/>
-      <c r="L77" s="4"/>
-    </row>
-    <row r="78" ht="14.25">
-      <c r="K78" s="4"/>
-      <c r="L78" s="4"/>
-    </row>
-    <row r="79" ht="14.25">
-      <c r="K79" s="4"/>
-      <c r="L79" s="4"/>
-    </row>
-    <row r="80" ht="14.25">
-      <c r="K80" s="4"/>
-      <c r="L80" s="4"/>
-    </row>
-    <row r="81" ht="14.25">
-      <c r="K81" s="4"/>
-      <c r="L81" s="4"/>
-    </row>
-    <row r="82" ht="14.25">
-      <c r="K82" s="4"/>
-      <c r="L82" s="4"/>
-    </row>
-    <row r="83" ht="14.25">
-      <c r="K83" s="4"/>
-      <c r="L83" s="4"/>
-    </row>
-    <row r="84" ht="14.25">
-      <c r="K84" s="4"/>
-      <c r="L84" s="4"/>
-    </row>
-    <row r="85" ht="14.25">
-      <c r="K85" s="4"/>
-      <c r="L85" s="4"/>
-    </row>
-    <row r="86" ht="14.25">
-      <c r="K86" s="4"/>
-      <c r="L86" s="4"/>
-    </row>
-    <row r="87" ht="14.25">
-      <c r="K87" s="4"/>
-      <c r="L87" s="4"/>
-    </row>
-    <row r="88" ht="14.25">
-      <c r="K88" s="4"/>
-      <c r="L88" s="4"/>
-    </row>
-    <row r="89" ht="14.25">
-      <c r="K89" s="4"/>
-      <c r="L89" s="4"/>
-    </row>
-    <row r="90" ht="14.25">
-      <c r="K90" s="4"/>
-      <c r="L90" s="4"/>
-    </row>
-    <row r="91" ht="14.25">
-      <c r="K91" s="4"/>
-      <c r="L91" s="4"/>
-    </row>
-    <row r="92" ht="14.25">
-      <c r="K92" s="4"/>
-      <c r="L92" s="4"/>
-    </row>
-    <row r="93" ht="14.25">
-      <c r="K93" s="4"/>
-      <c r="L93" s="4"/>
-    </row>
-    <row r="94" ht="14.25">
-      <c r="K94" s="4"/>
-      <c r="L94" s="4"/>
-    </row>
-    <row r="95" ht="14.25">
-      <c r="K95" s="4"/>
-      <c r="L95" s="4"/>
-    </row>
-    <row r="96" ht="14.25">
-      <c r="K96" s="4"/>
-      <c r="L96" s="4"/>
-    </row>
-    <row r="97" ht="14.25">
-      <c r="K97" s="4"/>
-      <c r="L97" s="4"/>
-    </row>
-    <row r="98" ht="14.25">
-      <c r="K98" s="4"/>
-      <c r="L98" s="4"/>
-    </row>
-    <row r="99" ht="14.25">
-      <c r="K99" s="4"/>
-      <c r="L99" s="4"/>
-    </row>
-    <row r="100" ht="14.25">
-      <c r="K100" s="4"/>
-      <c r="L100" s="4"/>
-    </row>
-    <row r="101" ht="14.25">
-      <c r="K101" s="4"/>
-      <c r="L101" s="4"/>
-    </row>
-    <row r="102" ht="14.25">
-      <c r="K102" s="4"/>
-      <c r="L102" s="4"/>
-    </row>
-    <row r="103" ht="14.25">
-      <c r="K103" s="4"/>
-      <c r="L103" s="4"/>
-    </row>
-    <row r="104" ht="14.25">
-      <c r="K104" s="4"/>
-      <c r="L104" s="4"/>
-    </row>
-    <row r="105" ht="14.25">
-      <c r="K105" s="4"/>
-      <c r="L105" s="4"/>
-    </row>
-    <row r="106" ht="14.25">
-      <c r="K106" s="4"/>
-      <c r="L106" s="4"/>
-    </row>
-    <row r="107" ht="14.25">
-      <c r="K107" s="4"/>
-      <c r="L107" s="4"/>
-    </row>
-    <row r="108" ht="14.25">
-      <c r="K108" s="4"/>
-      <c r="L108" s="4"/>
-    </row>
-    <row r="109" ht="14.25">
-      <c r="K109" s="4"/>
-      <c r="L109" s="4"/>
-    </row>
-    <row r="110" ht="14.25">
-      <c r="K110" s="4"/>
-      <c r="L110" s="4"/>
-    </row>
-    <row r="111" ht="14.25">
-      <c r="K111" s="4"/>
-      <c r="L111" s="4"/>
-    </row>
-    <row r="112" ht="14.25">
-      <c r="K112" s="4"/>
-      <c r="L112" s="4"/>
-    </row>
-    <row r="113" ht="14.25">
-      <c r="K113" s="4"/>
-      <c r="L113" s="4"/>
-    </row>
-    <row r="114" ht="14.25">
-      <c r="K114" s="4"/>
-      <c r="L114" s="4"/>
-    </row>
-    <row r="115" ht="14.25">
-      <c r="K115" s="4"/>
-      <c r="L115" s="4"/>
-    </row>
-    <row r="116" ht="14.25">
-      <c r="K116" s="4"/>
-      <c r="L116" s="4"/>
-    </row>
-    <row r="117" ht="14.25">
-      <c r="K117" s="4"/>
-      <c r="L117" s="4"/>
-    </row>
-    <row r="118" ht="14.25">
-      <c r="K118" s="4"/>
-      <c r="L118" s="4"/>
-    </row>
-    <row r="119" ht="14.25">
-      <c r="K119" s="4"/>
-      <c r="L119" s="4"/>
-    </row>
-    <row r="120" ht="14.25">
-      <c r="K120" s="4"/>
-      <c r="L120" s="4"/>
-    </row>
-    <row r="121" ht="14.25">
-      <c r="K121" s="4"/>
-      <c r="L121" s="4"/>
-    </row>
-    <row r="122" ht="14.25">
-      <c r="K122" s="4"/>
-      <c r="L122" s="4"/>
-    </row>
-    <row r="123" ht="14.25">
-      <c r="K123" s="4"/>
-      <c r="L123" s="4"/>
-    </row>
-    <row r="124" ht="14.25">
-      <c r="K124" s="6"/>
+      <c r="K52" s="2"/>
+      <c r="L52" s="2"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K53" s="2"/>
+      <c r="L53" s="2"/>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K54" s="2"/>
+      <c r="L54" s="2"/>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K55" s="2"/>
+      <c r="L55" s="2"/>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K56" s="2"/>
+      <c r="L56" s="2"/>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K57" s="2"/>
+      <c r="L57" s="2"/>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K58" s="2"/>
+      <c r="L58" s="2"/>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K59" s="2"/>
+      <c r="L59" s="2"/>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K60" s="2"/>
+      <c r="L60" s="2"/>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K61" s="2"/>
+      <c r="L61" s="2"/>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K62" s="2"/>
+      <c r="L62" s="2"/>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K63" s="2"/>
+      <c r="L63" s="2"/>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K64" s="2"/>
+      <c r="L64" s="2"/>
+    </row>
+    <row r="65" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K65" s="2"/>
+      <c r="L65" s="2"/>
+    </row>
+    <row r="66" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K66" s="2"/>
+      <c r="L66" s="2"/>
+    </row>
+    <row r="67" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K67" s="2"/>
+      <c r="L67" s="2"/>
+    </row>
+    <row r="68" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K68" s="2"/>
+      <c r="L68" s="2"/>
+    </row>
+    <row r="69" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K69" s="2"/>
+      <c r="L69" s="2"/>
+    </row>
+    <row r="70" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K70" s="2"/>
+      <c r="L70" s="2"/>
+    </row>
+    <row r="71" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K71" s="2"/>
+      <c r="L71" s="2"/>
+    </row>
+    <row r="72" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K72" s="2"/>
+      <c r="L72" s="2"/>
+    </row>
+    <row r="73" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K73" s="2"/>
+      <c r="L73" s="2"/>
+    </row>
+    <row r="74" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K74" s="2"/>
+      <c r="L74" s="2"/>
+    </row>
+    <row r="75" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K75" s="2"/>
+      <c r="L75" s="2"/>
+    </row>
+    <row r="76" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K76" s="2"/>
+      <c r="L76" s="2"/>
+    </row>
+    <row r="77" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K77" s="2"/>
+      <c r="L77" s="2"/>
+    </row>
+    <row r="78" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K78" s="2"/>
+      <c r="L78" s="2"/>
+    </row>
+    <row r="79" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K79" s="2"/>
+      <c r="L79" s="2"/>
+    </row>
+    <row r="80" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K80" s="2"/>
+      <c r="L80" s="2"/>
+    </row>
+    <row r="81" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K81" s="2"/>
+      <c r="L81" s="2"/>
+    </row>
+    <row r="82" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K82" s="2"/>
+      <c r="L82" s="2"/>
+    </row>
+    <row r="83" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K83" s="2"/>
+      <c r="L83" s="2"/>
+    </row>
+    <row r="84" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K84" s="2"/>
+      <c r="L84" s="2"/>
+    </row>
+    <row r="85" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K85" s="2"/>
+      <c r="L85" s="2"/>
+    </row>
+    <row r="86" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K86" s="2"/>
+      <c r="L86" s="2"/>
+    </row>
+    <row r="87" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K87" s="2"/>
+      <c r="L87" s="2"/>
+    </row>
+    <row r="88" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K88" s="2"/>
+      <c r="L88" s="2"/>
+    </row>
+    <row r="89" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K89" s="2"/>
+      <c r="L89" s="2"/>
+    </row>
+    <row r="90" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K90" s="2"/>
+      <c r="L90" s="2"/>
+    </row>
+    <row r="91" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K91" s="2"/>
+      <c r="L91" s="2"/>
+    </row>
+    <row r="92" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K92" s="2"/>
+      <c r="L92" s="2"/>
+    </row>
+    <row r="93" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K93" s="2"/>
+      <c r="L93" s="2"/>
+    </row>
+    <row r="94" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K94" s="2"/>
+      <c r="L94" s="2"/>
+    </row>
+    <row r="95" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K95" s="2"/>
+      <c r="L95" s="2"/>
+    </row>
+    <row r="96" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K96" s="2"/>
+      <c r="L96" s="2"/>
+    </row>
+    <row r="97" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K97" s="2"/>
+      <c r="L97" s="2"/>
+    </row>
+    <row r="98" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K98" s="2"/>
+      <c r="L98" s="2"/>
+    </row>
+    <row r="99" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K99" s="2"/>
+      <c r="L99" s="2"/>
+    </row>
+    <row r="100" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K100" s="2"/>
+      <c r="L100" s="2"/>
+    </row>
+    <row r="101" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K101" s="2"/>
+      <c r="L101" s="2"/>
+    </row>
+    <row r="102" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K102" s="2"/>
+      <c r="L102" s="2"/>
+    </row>
+    <row r="103" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K103" s="2"/>
+      <c r="L103" s="2"/>
+    </row>
+    <row r="104" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K104" s="2"/>
+      <c r="L104" s="2"/>
+    </row>
+    <row r="105" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K105" s="2"/>
+      <c r="L105" s="2"/>
+    </row>
+    <row r="106" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K106" s="2"/>
+      <c r="L106" s="2"/>
+    </row>
+    <row r="107" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K107" s="2"/>
+      <c r="L107" s="2"/>
+    </row>
+    <row r="108" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K108" s="2"/>
+      <c r="L108" s="2"/>
+    </row>
+    <row r="109" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K109" s="2"/>
+      <c r="L109" s="2"/>
+    </row>
+    <row r="110" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K110" s="2"/>
+      <c r="L110" s="2"/>
+    </row>
+    <row r="111" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K111" s="2"/>
+      <c r="L111" s="2"/>
+    </row>
+    <row r="112" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K112" s="2"/>
+      <c r="L112" s="2"/>
+    </row>
+    <row r="113" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K113" s="2"/>
+      <c r="L113" s="2"/>
+    </row>
+    <row r="114" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K114" s="2"/>
+      <c r="L114" s="2"/>
+    </row>
+    <row r="115" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K115" s="2"/>
+      <c r="L115" s="2"/>
+    </row>
+    <row r="116" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K116" s="2"/>
+      <c r="L116" s="2"/>
+    </row>
+    <row r="117" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K117" s="2"/>
+      <c r="L117" s="2"/>
+    </row>
+    <row r="118" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K118" s="2"/>
+      <c r="L118" s="2"/>
+    </row>
+    <row r="119" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K119" s="2"/>
+      <c r="L119" s="2"/>
+    </row>
+    <row r="120" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K120" s="2"/>
+      <c r="L120" s="2"/>
+    </row>
+    <row r="121" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K121" s="2"/>
+      <c r="L121" s="2"/>
+    </row>
+    <row r="122" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K122" s="2"/>
+      <c r="L122" s="2"/>
+    </row>
+    <row r="123" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K123" s="2"/>
+      <c r="L123" s="2"/>
+    </row>
+    <row r="124" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K124" s="3"/>
     </row>
   </sheetData>
-  <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
-      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
-      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>